<commit_message>
review submission with document
</commit_message>
<xml_diff>
--- a/src/test/resources/excelFile/ConsumerXpath.xlsx
+++ b/src/test/resources/excelFile/ConsumerXpath.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms185944\IdeaProjects\CambridgeTest\cucumber\src\test\resources\excelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDA7CA8-0670-4948-83EC-657BA95923EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E64D9F-206A-4BA7-9C25-1325979357D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -202,15 +202,9 @@
     <t>//tf-expansion-panel//[@t-model='Submission__c.PartyXrefs__r.%s']//tf-input[@t-model='City__c']/descendant::input</t>
   </si>
   <si>
-    <t>//tf-expansion-panel//[@t-model='Submission__c.PartyXrefs__r.%s']//tf-input[@t-model='ZipCode__c']/descendant::input</t>
-  </si>
-  <si>
     <t>//tf-expansion-panel//[@t-model='Submission__c.PartyXrefs__r.%s']//tf-phone[@t-model='Party__r.PrimaryPhone__c']/descendant::input</t>
   </si>
   <si>
-    <t>//tf-expansion-panel//[@t-model='Submission__c.PartyXrefs__r.%s']//tf-phone[@t-model='Party__r.SecondaryPhone__c']/descendant::input</t>
-  </si>
-  <si>
     <t>//tf-expansion-panel//[@t-model='Submission__c.PartyXrefs__r.%s']//tf-dropdown[@t-model='Type__c']/descendant::input</t>
   </si>
   <si>
@@ -617,6 +611,12 @@
   </si>
   <si>
     <t>//tf-expansion-panel//div[@t-model='Submission__c.PartyXrefs__r.%s']//tf-dropdown[@t-model='State__c']/descendant::input</t>
+  </si>
+  <si>
+    <t>//tf-expansion-panel//div[@t-model='Submission__c.PartyXrefs__r.%s']//tf-input[@t-model='ZipCode__c']/descendant::input</t>
+  </si>
+  <si>
+    <t>//tf-expansion-panel//div[@t-model='Submission__c.PartyXrefs__r.%s']//tf-phone[@t-model='Party__r.PrimaryPhone__c']//input</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1187,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>13</v>
@@ -1405,7 +1405,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>6</v>
@@ -1493,7 +1493,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>57</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1524,10 +1524,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,10 +1541,10 @@
         <v>21</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
         <v>58</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,7 +1578,7 @@
         <v>59</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1592,10 +1592,10 @@
         <v>40</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1609,10 +1609,10 @@
         <v>21</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>60</v>
+        <v>197</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1626,10 +1626,10 @@
         <v>40</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1643,10 +1643,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1660,10 +1660,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1677,10 +1677,10 @@
         <v>25</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1694,10 +1694,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1726,10 +1726,10 @@
         <v>50</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1743,10 +1743,10 @@
         <v>40</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1760,10 +1760,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1792,10 +1792,10 @@
         <v>55</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1809,10 +1809,10 @@
         <v>55</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <v>35</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>6</v>
@@ -1834,16 +1834,16 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>6</v>
@@ -1851,16 +1851,16 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>6</v>
@@ -1868,16 +1868,16 @@
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>6</v>
@@ -1885,16 +1885,16 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>6</v>
@@ -1902,16 +1902,16 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>6</v>
@@ -1919,16 +1919,16 @@
     </row>
     <row r="40" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>6</v>
@@ -1936,16 +1936,16 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>40</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>6</v>
@@ -1953,16 +1953,16 @@
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E42" s="20" t="s">
         <v>6</v>
@@ -1970,16 +1970,16 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>6</v>
@@ -1987,16 +1987,16 @@
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E44" s="20" t="s">
         <v>6</v>
@@ -2004,16 +2004,16 @@
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>6</v>
@@ -2021,16 +2021,16 @@
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>6</v>
@@ -2038,16 +2038,16 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>6</v>
@@ -2055,16 +2055,16 @@
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B48" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="20" t="s">
         <v>95</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>97</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>6</v>
@@ -2072,16 +2072,16 @@
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>6</v>
@@ -2089,16 +2089,16 @@
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>6</v>
@@ -2106,16 +2106,16 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>6</v>
@@ -2123,16 +2123,16 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>6</v>
@@ -2140,16 +2140,16 @@
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>6</v>
@@ -2157,16 +2157,16 @@
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E54" s="20" t="s">
         <v>6</v>
@@ -2174,16 +2174,16 @@
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>40</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E55" s="13" t="s">
         <v>6</v>
@@ -2191,16 +2191,16 @@
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>6</v>
@@ -2208,16 +2208,16 @@
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B57" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>116</v>
       </c>
       <c r="E57" s="13" t="s">
         <v>6</v>
@@ -2225,16 +2225,16 @@
     </row>
     <row r="58" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>6</v>
@@ -2242,16 +2242,16 @@
     </row>
     <row r="59" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>6</v>
@@ -2259,16 +2259,16 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>6</v>
@@ -2276,16 +2276,16 @@
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E61" s="13" t="s">
         <v>6</v>
@@ -2293,16 +2293,16 @@
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C62" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E62" s="20" t="s">
         <v>6</v>
@@ -2310,16 +2310,16 @@
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E63" s="13" t="s">
         <v>6</v>
@@ -2327,16 +2327,16 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>6</v>
@@ -2344,16 +2344,16 @@
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>6</v>
@@ -2361,16 +2361,16 @@
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C66" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>6</v>
@@ -2378,16 +2378,16 @@
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E67" s="13" t="s">
         <v>6</v>
@@ -2395,16 +2395,16 @@
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C68" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E68" s="20" t="s">
         <v>6</v>
@@ -2412,16 +2412,16 @@
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E69" s="13" t="s">
         <v>6</v>
@@ -2429,16 +2429,16 @@
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C70" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E70" s="20" t="s">
         <v>6</v>
@@ -2446,16 +2446,16 @@
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E71" s="13" t="s">
         <v>6</v>
@@ -2463,16 +2463,16 @@
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E72" s="20" t="s">
         <v>6</v>
@@ -2480,16 +2480,16 @@
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E73" s="13" t="s">
         <v>6</v>
@@ -2497,16 +2497,16 @@
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E74" s="20" t="s">
         <v>6</v>
@@ -2514,16 +2514,16 @@
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E75" s="13" t="s">
         <v>6</v>
@@ -2531,10 +2531,10 @@
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>13</v>
@@ -2548,16 +2548,16 @@
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E77" s="13" t="s">
         <v>6</v>
@@ -2565,16 +2565,16 @@
     </row>
     <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C78" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E78" s="20" t="s">
         <v>6</v>
@@ -2582,16 +2582,16 @@
     </row>
     <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E79" s="13" t="s">
         <v>6</v>
@@ -2599,33 +2599,33 @@
     </row>
     <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C80" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E80" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E81" s="20" t="s">
         <v>6</v>
@@ -2633,16 +2633,16 @@
     </row>
     <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B82" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C82" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E82" s="20" t="s">
         <v>6</v>
@@ -2650,16 +2650,16 @@
     </row>
     <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E83" s="20" t="s">
         <v>6</v>
@@ -2667,16 +2667,16 @@
     </row>
     <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C84" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E84" s="20" t="s">
         <v>6</v>
@@ -2684,16 +2684,16 @@
     </row>
     <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E85" s="20" t="s">
         <v>6</v>
@@ -2701,16 +2701,16 @@
     </row>
     <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B86" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C86" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D86" s="20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E86" s="20" t="s">
         <v>6</v>
@@ -2718,16 +2718,16 @@
     </row>
     <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E87" s="20" t="s">
         <v>6</v>
@@ -2735,33 +2735,33 @@
     </row>
     <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E88" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C89" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E89" s="20" t="s">
         <v>6</v>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B90" s="20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C90" s="18" t="s">
         <v>13</v>
@@ -2786,16 +2786,16 @@
     </row>
     <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C91" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E91" s="20" t="s">
         <v>6</v>
@@ -2803,16 +2803,16 @@
     </row>
     <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C92" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D92" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E92" s="20" t="s">
         <v>6</v>
@@ -2820,16 +2820,16 @@
     </row>
     <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C93" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>6</v>

</xml_diff>